<commit_message>
Creating and updating plots
</commit_message>
<xml_diff>
--- a/data/Wallkill_2018/Wallkill_2018_flow_fieldsheets.xlsx
+++ b/data/Wallkill_2018/Wallkill_2018_flow_fieldsheets.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\parameterized_reports\data\Wallkill_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ABCEB1-EE28-4CB9-8FBC-9990FCECB5BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0143F6B8-AD71-4CB2-9DFB-E0C20D62EB53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10110" activeTab="1" xr2:uid="{9096190B-EA1F-4934-B501-C3476D4BCA25}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10110" xr2:uid="{9096190B-EA1F-4934-B501-C3476D4BCA25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Flow" sheetId="2" r:id="rId1"/>
+    <sheet name="flow" sheetId="2" r:id="rId1"/>
     <sheet name="simplified qual" sheetId="4" r:id="rId2"/>
     <sheet name="pivot" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$I$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flow!$A$1:$I$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="60">
   <si>
     <t>13-DWAR-2.0</t>
   </si>
@@ -100,18 +100,9 @@
     <t>13-WKLEI-0.6</t>
   </si>
   <si>
-    <t>SiteID</t>
-  </si>
-  <si>
     <t>baseline</t>
   </si>
   <si>
-    <t>Flow_qual</t>
-  </si>
-  <si>
-    <t>Flow_quant_cfs</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>Uncertainty</t>
   </si>
   <si>
-    <t>Sample_date</t>
-  </si>
-  <si>
     <t>Highest_error_src_pct_err</t>
   </si>
   <si>
@@ -224,6 +212,12 @@
   </si>
   <si>
     <t>flow_qual</t>
+  </si>
+  <si>
+    <t>flow_quant_cfs</t>
+  </si>
+  <si>
+    <t>station</t>
   </si>
 </sst>
 </file>
@@ -302,7 +296,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gavin Lemley" refreshedDate="43579.663187962964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="76" xr:uid="{8226D2A4-B3DE-4A40-B696-88D49C865E9D}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I79" sheet="Flow"/>
+    <worksheetSource ref="A1:I79" sheet="flow"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="SiteID" numFmtId="0">
@@ -1422,9 +1416,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEA01C-0BB2-463B-AB1C-7F63247689C4}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,31 +1435,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1476,10 +1470,10 @@
         <v>43291</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5">
         <v>5.4240000000000004</v>
@@ -1497,10 +1491,10 @@
         <v>43291</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5">
         <v>33.747999999999998</v>
@@ -1518,10 +1512,10 @@
         <v>43291</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5">
         <v>1.609</v>
@@ -1539,10 +1533,10 @@
         <v>43291</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5">
         <v>1.62</v>
@@ -1560,10 +1554,10 @@
         <v>43292</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5">
         <v>1.4999999999999999E-2</v>
@@ -1581,10 +1575,10 @@
         <v>43292</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -1594,16 +1588,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6">
         <v>43292</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5">
         <v>0.46400000000000002</v>
@@ -1621,10 +1615,10 @@
         <v>43292</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5">
         <v>0.159</v>
@@ -1642,10 +1636,10 @@
         <v>43292</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="5">
         <v>0.28999999999999998</v>
@@ -1663,10 +1657,10 @@
         <v>43292</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="5">
         <v>1.754</v>
@@ -1684,10 +1678,10 @@
         <v>43292</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="5">
         <v>0.78</v>
@@ -1705,10 +1699,10 @@
         <v>43292</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5">
         <v>1.2</v>
@@ -1726,10 +1720,10 @@
         <v>43292</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5">
         <v>1.2989999999999999</v>
@@ -1747,10 +1741,10 @@
         <v>43292</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="5">
         <v>1.94</v>
@@ -1768,10 +1762,10 @@
         <v>43292</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="5">
         <v>0.79500000000000004</v>
@@ -1789,10 +1783,10 @@
         <v>43292</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="5">
         <v>0.247</v>
@@ -1810,10 +1804,10 @@
         <v>43305</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1829,10 +1823,10 @@
         <v>43305</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="5">
         <v>35.497999999999998</v>
@@ -1850,17 +1844,17 @@
         <v>43305</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1871,17 +1865,17 @@
         <v>43305</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1892,10 +1886,10 @@
         <v>43305</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="5">
         <v>156.215</v>
@@ -1904,7 +1898,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1915,10 +1909,10 @@
         <v>43305</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5">
         <v>4.57</v>
@@ -1927,7 +1921,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,10 +1932,10 @@
         <v>43305</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" s="7">
         <v>37.29</v>
@@ -1959,10 +1953,10 @@
         <v>43305</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E25" s="5">
         <v>34.228999999999999</v>
@@ -1971,7 +1965,7 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1982,10 +1976,10 @@
         <v>43306</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5">
         <v>8.3109999999999999</v>
@@ -2003,10 +1997,10 @@
         <v>43306</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E27" s="5">
         <v>16.663</v>
@@ -2018,16 +2012,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28" s="6">
         <v>43306</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E28" s="5">
         <v>16.285</v>
@@ -2045,10 +2039,10 @@
         <v>43306</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E29" s="5">
         <v>0.87</v>
@@ -2066,10 +2060,10 @@
         <v>43306</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E30" s="5">
         <v>30.033000000000001</v>
@@ -2087,10 +2081,10 @@
         <v>43306</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E31" s="5">
         <v>72.757000000000005</v>
@@ -2108,10 +2102,10 @@
         <v>43306</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E32" s="5">
         <v>23.067</v>
@@ -2129,10 +2123,10 @@
         <v>43306</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E33" s="5">
         <v>8.2110000000000003</v>
@@ -2150,17 +2144,17 @@
         <v>43306</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2171,17 +2165,17 @@
         <v>43306</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2192,10 +2186,10 @@
         <v>43306</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5">
         <v>12.265000000000001</v>
@@ -2213,10 +2207,10 @@
         <v>43326</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E37" s="5">
         <v>17.966000000000001</v>
@@ -2225,7 +2219,7 @@
         <v>12.6</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H37" s="5">
         <v>11.6</v>
@@ -2240,10 +2234,10 @@
         <v>43326</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E38" s="5">
         <v>366.82400000000001</v>
@@ -2252,13 +2246,13 @@
         <v>5.3</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H38" s="5">
         <v>5</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2269,10 +2263,10 @@
         <v>43326</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E39" s="5">
         <v>14.375</v>
@@ -2281,7 +2275,7 @@
         <v>10.7</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H39" s="5">
         <v>9.3000000000000007</v>
@@ -2296,10 +2290,10 @@
         <v>43326</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E40" s="5">
         <v>17.503</v>
@@ -2308,7 +2302,7 @@
         <v>6.5</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H40" s="5">
         <v>5.0999999999999996</v>
@@ -2323,10 +2317,10 @@
         <v>43327</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E41" s="5">
         <v>54.786999999999999</v>
@@ -2344,10 +2338,10 @@
         <v>43327</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E42" s="5">
         <v>23.821999999999999</v>
@@ -2356,7 +2350,7 @@
         <v>12.3</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H42" s="5">
         <v>11.8</v>
@@ -2371,10 +2365,10 @@
         <v>43327</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E43" s="5">
         <v>33.609000000000002</v>
@@ -2383,7 +2377,7 @@
         <v>6.2</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H43" s="5">
         <v>5.4</v>
@@ -2398,10 +2392,10 @@
         <v>43327</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E44" s="5">
         <v>33.863</v>
@@ -2419,10 +2413,10 @@
         <v>43327</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E45" s="5">
         <v>54.585000000000001</v>
@@ -2440,10 +2434,10 @@
         <v>43327</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E46" s="5">
         <v>16.140999999999998</v>
@@ -2452,7 +2446,7 @@
         <v>2.9</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H46" s="5">
         <v>2.2999999999999998</v>
@@ -2467,10 +2461,10 @@
         <v>43328</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E47" s="5">
         <v>2.3580000000000001</v>
@@ -2488,10 +2482,10 @@
         <v>43328</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E48" s="5">
         <v>11.702999999999999</v>
@@ -2503,16 +2497,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B49" s="6">
         <v>43328</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E49" s="5">
         <v>13.382</v>
@@ -2530,10 +2524,10 @@
         <v>43328</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E50" s="5">
         <v>0.42</v>
@@ -2551,10 +2545,10 @@
         <v>43328</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E51" s="5">
         <v>8.84</v>
@@ -2572,10 +2566,10 @@
         <v>43348</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E52" s="5">
         <v>0.41499999999999998</v>
@@ -2593,10 +2587,10 @@
         <v>43348</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E53" s="5">
         <v>0.11899999999999999</v>
@@ -2608,16 +2602,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B54" s="6">
         <v>43348</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E54" s="5">
         <v>0.746</v>
@@ -2635,10 +2629,10 @@
         <v>43348</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" s="5">
         <v>0.29199999999999998</v>
@@ -2656,10 +2650,10 @@
         <v>43348</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E56" s="5">
         <v>1.847</v>
@@ -2677,10 +2671,10 @@
         <v>43348</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E57" s="5">
         <v>78.158000000000001</v>
@@ -2689,7 +2683,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2700,10 +2694,10 @@
         <v>43348</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" s="5">
         <v>14.561999999999999</v>
@@ -2712,7 +2706,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2723,10 +2717,10 @@
         <v>43348</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E59" s="5">
         <v>14.3</v>
@@ -2735,7 +2729,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2746,10 +2740,10 @@
         <v>43348</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E60" s="5">
         <v>1.7250000000000001</v>
@@ -2758,7 +2752,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2769,10 +2763,10 @@
         <v>43348</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E61" s="5">
         <v>0.56899999999999995</v>
@@ -2781,7 +2775,7 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2792,10 +2786,10 @@
         <v>43349</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E62" s="5">
         <v>2.9350000000000001</v>
@@ -2813,10 +2807,10 @@
         <v>43349</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E63" s="5">
         <v>40.411000000000001</v>
@@ -2834,10 +2828,10 @@
         <v>43349</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E64" s="5">
         <v>1.0549999999999999</v>
@@ -2846,7 +2840,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2857,10 +2851,10 @@
         <v>43349</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E65" s="5">
         <v>3.129</v>
@@ -2869,7 +2863,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2880,10 +2874,10 @@
         <v>43349</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E66" s="5">
         <v>1.696</v>
@@ -2901,10 +2895,10 @@
         <v>43349</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E67" s="5">
         <v>2.198</v>
@@ -2913,7 +2907,7 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2924,10 +2918,10 @@
         <v>43349</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E68" s="5">
         <v>5.3159999999999998</v>
@@ -2945,10 +2939,10 @@
         <v>43349</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E69" s="5">
         <v>1.2310000000000001</v>
@@ -2957,7 +2951,7 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2968,10 +2962,10 @@
         <v>43375</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E70" s="5">
         <v>43.475999999999999</v>
@@ -2989,10 +2983,10 @@
         <v>43375</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E71" s="5">
         <v>50.734999999999999</v>
@@ -3010,10 +3004,10 @@
         <v>43375</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E72" s="5">
         <v>50.155000000000001</v>
@@ -3031,10 +3025,10 @@
         <v>43376</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E73" s="5">
         <v>13.89</v>
@@ -3052,10 +3046,10 @@
         <v>43376</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E74" s="5">
         <v>63.38</v>
@@ -3067,16 +3061,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B75" s="6">
         <v>43376</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E75" s="5">
         <v>37.438000000000002</v>
@@ -3094,10 +3088,10 @@
         <v>43376</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E76" s="5">
         <v>11.48</v>
@@ -3115,10 +3109,10 @@
         <v>43376</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E77" s="5">
         <v>34.76</v>
@@ -3136,10 +3130,10 @@
         <v>43377</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E78" s="5">
         <v>29.056999999999999</v>
@@ -3148,13 +3142,13 @@
         <v>3.2</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H78" s="5">
         <v>2.9</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3165,10 +3159,10 @@
         <v>43377</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E79" s="5">
         <v>43.448999999999998</v>
@@ -3177,13 +3171,13 @@
         <v>3.9</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H79" s="5">
         <v>3.6</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3199,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E72531-21E7-428E-BD05-0438918E28DA}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3211,10 +3205,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3222,7 +3216,7 @@
         <v>43291</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3230,7 +3224,7 @@
         <v>43292</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3238,7 +3232,7 @@
         <v>43305</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3246,7 +3240,7 @@
         <v>43306</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3254,7 +3248,7 @@
         <v>43326</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3262,7 +3256,7 @@
         <v>43327</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3270,7 +3264,7 @@
         <v>43328</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3278,7 +3272,7 @@
         <v>43348</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3286,7 +3280,7 @@
         <v>43349</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3294,7 +3288,7 @@
         <v>43375</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3302,7 +3296,7 @@
         <v>43376</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3310,7 +3304,7 @@
         <v>43377</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3334,10 +3328,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3374,7 +3368,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
@@ -3510,7 +3504,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3">
         <v>76</v>

</xml_diff>

<commit_message>
Creating plots using functions.
</commit_message>
<xml_diff>
--- a/data/Wallkill_2018/Wallkill_2018_flow_fieldsheets.xlsx
+++ b/data/Wallkill_2018/Wallkill_2018_flow_fieldsheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\parameterized_reports\data\Wallkill_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0143F6B8-AD71-4CB2-9DFB-E0C20D62EB53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD85AFF-C764-4FA5-B8B6-5095D8769B77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10110" xr2:uid="{9096190B-EA1F-4934-B501-C3476D4BCA25}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="60">
   <si>
     <t>13-DWAR-2.0</t>
   </si>
@@ -262,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -276,6 +276,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,7 +1418,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -3191,20 +3192,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E72531-21E7-428E-BD05-0438918E28DA}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B1" t="s">
@@ -3307,8 +3308,89 @@
         <v>22</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>42935</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>42936</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>42948</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>42949</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>42984</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>42985</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>42997</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>42998</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>43019</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>43020</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>